<commit_message>
Finished calculations for unit testing
</commit_message>
<xml_diff>
--- a/unit_tests_manual_calculations.xlsx
+++ b/unit_tests_manual_calculations.xlsx
@@ -9,10 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Explicit Euler" sheetId="1" r:id="rId1"/>
+    <sheet name="Verlet" sheetId="2" r:id="rId2"/>
+    <sheet name="Midpoint" sheetId="3" r:id="rId3"/>
+    <sheet name="RK4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="246">
   <si>
     <t>T0</t>
   </si>
@@ -237,6 +240,531 @@
   </si>
   <si>
     <t>(-2, -0.7468, 0)</t>
+  </si>
+  <si>
+    <t>Total force</t>
+  </si>
+  <si>
+    <t>(11.4623442, -42.3819427, 0)</t>
+  </si>
+  <si>
+    <t>(0, -8.68060398, 0)</t>
+  </si>
+  <si>
+    <t>(-11.4623442, -42.3819427, 0)</t>
+  </si>
+  <si>
+    <t>(0, 9.80999851, 0)</t>
+  </si>
+  <si>
+    <t>(0, 13.0024862, 0)</t>
+  </si>
+  <si>
+    <t>(0, -8.82900047, 0)</t>
+  </si>
+  <si>
+    <t>(0, -9.81000042, 0)</t>
+  </si>
+  <si>
+    <t>(0, -0.868060398, 0)</t>
+  </si>
+  <si>
+    <t>(0, 0.980999851, 0)</t>
+  </si>
+  <si>
+    <t>(0, 1.30024862, 0)</t>
+  </si>
+  <si>
+    <t>(0, -0.882900047, 0)</t>
+  </si>
+  <si>
+    <t>(0, -0.981000042, 0)</t>
+  </si>
+  <si>
+    <t>New Position</t>
+  </si>
+  <si>
+    <t>(-6, 7.174844602, 0)</t>
+  </si>
+  <si>
+    <t>(-10, 5.023902, 0)</t>
+  </si>
+  <si>
+    <t>(-6, 5.34319862, 0)</t>
+  </si>
+  <si>
+    <t>(-2, 5.023905, 0)</t>
+  </si>
+  <si>
+    <t>(-10, -8.39950047, 0)</t>
+  </si>
+  <si>
+    <t>(-6, -1.957050042, 0)</t>
+  </si>
+  <si>
+    <t>(-2, -8.33950047, 0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T0 </t>
+  </si>
+  <si>
+    <t>First int.</t>
+  </si>
+  <si>
+    <t>(0, -0.4905, 0)</t>
+  </si>
+  <si>
+    <t>Second int</t>
+  </si>
+  <si>
+    <t>Particle force</t>
+  </si>
+  <si>
+    <t>(0, 0.437500000, 0)</t>
+  </si>
+  <si>
+    <t>(0, -9.31951046, 0)</t>
+  </si>
+  <si>
+    <t>(0, -9.81000996, 0)</t>
+  </si>
+  <si>
+    <t>(0, -9.77324772, 0)</t>
+  </si>
+  <si>
+    <t>(0, -0.488662386, 0)</t>
+  </si>
+  <si>
+    <t>(3.371747425e-7, 1.23977661e-6, 0)</t>
+  </si>
+  <si>
+    <t>(6.74349485e-6, 2.47955322e-5, 0)</t>
+  </si>
+  <si>
+    <t>(-6.74349485e-6, 2.47955322e-5, 0)</t>
+  </si>
+  <si>
+    <t>(0, 0.021875, 0)</t>
+  </si>
+  <si>
+    <t>(-3.371747425e-7, 1.23977661e-6, 0)</t>
+  </si>
+  <si>
+    <t>(0, -0.4659575523, 0)</t>
+  </si>
+  <si>
+    <t>(0, -.468625, 0)</t>
+  </si>
+  <si>
+    <t>(-3.371747425e-7, -4.904987602, 0)</t>
+  </si>
+  <si>
+    <t>(0, -0.9564575523, 0)</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>(0, -0.979162386, 0)</t>
+  </si>
+  <si>
+    <t>(-6, 9.75475, 10)</t>
+  </si>
+  <si>
+    <t>(-10, 5.75475, 10)</t>
+  </si>
+  <si>
+    <t>(-6, 5.75475, 10)</t>
+  </si>
+  <si>
+    <t>(-2, 5.75475, 10)</t>
+  </si>
+  <si>
+    <t>(-10, 1.75475, 10)</t>
+  </si>
+  <si>
+    <t>(-6, 1.75475, 10)</t>
+  </si>
+  <si>
+    <t>(-2, 1.75475, 10)</t>
+  </si>
+  <si>
+    <t>(-6, 9.265168807, 0)</t>
+  </si>
+  <si>
+    <t>(3.371747425e-7, -0.4904987602, 0)</t>
+  </si>
+  <si>
+    <t>(-9.9999999831, 5.50950062, 0)</t>
+  </si>
+  <si>
+    <t>(-2.0000000831, 5.50950062, 0)</t>
+  </si>
+  <si>
+    <t>(-6, 5.5204375, 0)</t>
+  </si>
+  <si>
+    <t>(-10, 1.276521224, 0)</t>
+  </si>
+  <si>
+    <t>(-2, 1.276521224, 0)</t>
+  </si>
+  <si>
+    <t>(-6, 1.26425, 0)</t>
+  </si>
+  <si>
+    <t>(-1.38282776e-5, 10.6781187, 0)</t>
+  </si>
+  <si>
+    <t>(-0.130381584, -9.28915501, 0)</t>
+  </si>
+  <si>
+    <t>(0, -19.6512871, 0)</t>
+  </si>
+  <si>
+    <t>(0.130409718, -9.28915405, 0)</t>
+  </si>
+  <si>
+    <t>(4.80282927, 6.05143070, 0)</t>
+  </si>
+  <si>
+    <t>(-4.80282974, 6.05143070, 0)</t>
+  </si>
+  <si>
+    <t>K1</t>
+  </si>
+  <si>
+    <t>K2</t>
+  </si>
+  <si>
+    <t>Third int</t>
+  </si>
+  <si>
+    <t>Particle Force</t>
+  </si>
+  <si>
+    <t>(-6.9141388e-7, 0.533905935, 0)</t>
+  </si>
+  <si>
+    <t>(-6.9141388e-7, -.445256451, 0)</t>
+  </si>
+  <si>
+    <t>(-6, 9.042540582, 0)</t>
+  </si>
+  <si>
+    <t>(-6.5190792e-3, -0.4644577505, 0)</t>
+  </si>
+  <si>
+    <t>(-6.518742025e-3, -0.9549565107, 0)</t>
+  </si>
+  <si>
+    <t>(-10.00325935, 5.032022365, 0)</t>
+  </si>
+  <si>
+    <t>(0, -0.982564355, 0)</t>
+  </si>
+  <si>
+    <t>(0, -1.451189355, 0)</t>
+  </si>
+  <si>
+    <t>(-6, 4.794842823, 10)</t>
+  </si>
+  <si>
+    <t>(6.5204859e-3, -0.4644577025, 0)</t>
+  </si>
+  <si>
+    <t>(-3.371747425e-7, -0.4904987602, 0)</t>
+  </si>
+  <si>
+    <t>(6.520148725e-3, -0.9549564627, 0)</t>
+  </si>
+  <si>
+    <t>(-1.996739926, 5.032022389, 10)</t>
+  </si>
+  <si>
+    <t>(0.2401414635, 0.302571535, 0)</t>
+  </si>
+  <si>
+    <t>(0.2401414635, -0.6538860173, 0)</t>
+  </si>
+  <si>
+    <t>(-9.879929268, 0.9495782154, 10)</t>
+  </si>
+  <si>
+    <t>(-1.28746033e-005, 10.6868353, 0)</t>
+  </si>
+  <si>
+    <t>(-6.43730165e-7, 0.534341765, 0)</t>
+  </si>
+  <si>
+    <t>(-6.43730165e-7, -.446658235, 0)</t>
+  </si>
+  <si>
+    <t>(-6.000000322, 1.040920883, 10)</t>
+  </si>
+  <si>
+    <t>(-0.240141487, 0.302571535, 0)</t>
+  </si>
+  <si>
+    <t>(-0.240141487, -0.6538860173, 0)</t>
+  </si>
+  <si>
+    <t>(-2.120070744, 0.9495782154, 10)</t>
+  </si>
+  <si>
+    <t>K3</t>
+  </si>
+  <si>
+    <t>Fourth int</t>
+  </si>
+  <si>
+    <t>(5.94258308e-005, -18.2553787, 0)</t>
+  </si>
+  <si>
+    <t>(2.97129154e-6, -0.912768935, 0)</t>
+  </si>
+  <si>
+    <t>(-5.99999886, 8.363527889, 10)</t>
+  </si>
+  <si>
+    <t>(2.27987766e-6, -1.358025386, 0)</t>
+  </si>
+  <si>
+    <t>(0.713213325, 25.6412811, 0)</t>
+  </si>
+  <si>
+    <t>(0.03566066625, 1.282064055, 0)</t>
+  </si>
+  <si>
+    <t>(0.02914192423, 0.3271075443, 0)</t>
+  </si>
+  <si>
+    <t>(-9.988688388, 5.195576137, 10)</t>
+  </si>
+  <si>
+    <t>(4.76837158e-007, 78.5084686, 0)</t>
+  </si>
+  <si>
+    <t>(2.38418579e-8, 3.92542343, 0)</t>
+  </si>
+  <si>
+    <t>(2.38418579e-8, 2.474234075 0)</t>
+  </si>
+  <si>
+    <t>(-5.999999988, 6.031959861, 10)</t>
+  </si>
+  <si>
+    <t>(-0.713241577, 25.6412811, 0)</t>
+  </si>
+  <si>
+    <t>(-0.03566207885, 1.282064055, 0)</t>
+  </si>
+  <si>
+    <t>(-0.02914193013, 0.3271075923, 0)</t>
+  </si>
+  <si>
+    <t>(-2.011310891, 5.195576185, 10)</t>
+  </si>
+  <si>
+    <t>(-10.8820877, -10.3119888, 0)</t>
+  </si>
+  <si>
+    <t>(-.544104385, -0.51559944, 0)</t>
+  </si>
+  <si>
+    <t>(-0.3039629215, -1.169485457, 0)</t>
+  </si>
+  <si>
+    <t>(-10.03191073, 0.3648354869, 10)</t>
+  </si>
+  <si>
+    <t>(4.06727195e-5, -19.6507816, 0)</t>
+  </si>
+  <si>
+    <t>(2.033635975e-6, -0.98253908, 0)</t>
+  </si>
+  <si>
+    <t>(1.38990581e-6, -1.429197315, 0)</t>
+  </si>
+  <si>
+    <t>(-5.999999627, 0.3263222255, 10)</t>
+  </si>
+  <si>
+    <t>(10.8820581, -10.3119879, 0)</t>
+  </si>
+  <si>
+    <t>(0.544102905, -0.515599395, 0)</t>
+  </si>
+  <si>
+    <t>(0.303961418, -1.16985412, 0)</t>
+  </si>
+  <si>
+    <t>(-1.968090035, 0.3646511554, 10)</t>
+  </si>
+  <si>
+    <t>Final step</t>
+  </si>
+  <si>
+    <t>Original</t>
+  </si>
+  <si>
+    <t>K4</t>
+  </si>
+  <si>
+    <t>2K2</t>
+  </si>
+  <si>
+    <t>(0, -19.54649544, 0)</t>
+  </si>
+  <si>
+    <t>(1.34869897e-5, 4.95910644e-5, 0)</t>
+  </si>
+  <si>
+    <t>(0, -18.63902092, 0)</t>
+  </si>
+  <si>
+    <t>(0, 0.875, 0)</t>
+  </si>
+  <si>
+    <t>(0, -19.62001992, 0)</t>
+  </si>
+  <si>
+    <t>(-1.34869897e-5, 4.95910644e-5, 0)</t>
+  </si>
+  <si>
+    <t>2K3</t>
+  </si>
+  <si>
+    <t>(-2.76565552e-5, 21.3562374, 0)</t>
+  </si>
+  <si>
+    <t>(0, -39.3025742, 0)</t>
+  </si>
+  <si>
+    <t>(-2.57492066e-005, 21.3736706, 0)</t>
+  </si>
+  <si>
+    <t>(-0.260763168, -18.57831002, 0)</t>
+  </si>
+  <si>
+    <t>(9.60565854, 12.1028614, 0)</t>
+  </si>
+  <si>
+    <t>(0.260819432, -18.5783081, 0)</t>
+  </si>
+  <si>
+    <t>(-9.60565948, 12.1028614, 0)</t>
+  </si>
+  <si>
+    <t>K1 + 2K2</t>
+  </si>
+  <si>
+    <t>(0, -29.35649544, 0)</t>
+  </si>
+  <si>
+    <t>(1.34869897e-5, -9.809950409, 0)</t>
+  </si>
+  <si>
+    <t>(0, -8.935, 0)</t>
+  </si>
+  <si>
+    <t>(-1.34869897e-5, -9.809950409, 0)</t>
+  </si>
+  <si>
+    <t>(0, -28.44902092, 0)</t>
+  </si>
+  <si>
+    <t>(0, -29.43001992, 0)</t>
+  </si>
+  <si>
+    <t>2K3 + K4</t>
+  </si>
+  <si>
+    <t>(3.17692756e-5, 3.1008587, 0)</t>
+  </si>
+  <si>
+    <t>(0.452450157, 7.06297108, 0)</t>
+  </si>
+  <si>
+    <t>(4.76837158e-7, 39.2058941, 0)</t>
+  </si>
+  <si>
+    <t>(-0.452422145, 7.062973, 0)</t>
+  </si>
+  <si>
+    <t>(-1.27642916, 1.7908734, 0)</t>
+  </si>
+  <si>
+    <t>(1.49235129e-5, 1.722889, 0)</t>
+  </si>
+  <si>
+    <t>(1.27639862, 1.7908735, 0)</t>
+  </si>
+  <si>
+    <t>(K1+2K2) + (2K3+k4)</t>
+  </si>
+  <si>
+    <t>(3.17692756e-5, -26.25563674, 0)</t>
+  </si>
+  <si>
+    <t>(0.452463644, -2.746979326, 0)</t>
+  </si>
+  <si>
+    <t>(4.76837158e-7, 30.2708941, 0)</t>
+  </si>
+  <si>
+    <t>(-0.452435632, -2.746977409, 0)</t>
+  </si>
+  <si>
+    <t>(-1.27642916, -26.65814752, 0)</t>
+  </si>
+  <si>
+    <t>(1.49235129e-5, -27.70713092, 0)</t>
+  </si>
+  <si>
+    <t>(1.27639862, -26.65814742, 0)</t>
+  </si>
+  <si>
+    <t>(5.29487933e-7, -0.4375939457, 0)</t>
+  </si>
+  <si>
+    <t>(7.541060733e-3, -0.04578298877, 0)</t>
+  </si>
+  <si>
+    <t>(7.947285967e-9, 0.5045149017, 0)</t>
+  </si>
+  <si>
+    <t>(-7.540593867e-3, -0.04578295682, 0)</t>
+  </si>
+  <si>
+    <t>(-0.02127381933, -0.4443024587, 0)</t>
+  </si>
+  <si>
+    <t>(2.48725215e-7, -0.4617855153, 0)</t>
+  </si>
+  <si>
+    <t>(0.02127331033, -0.444302457, 0)</t>
+  </si>
+  <si>
+    <t>(-5.999999471, 9.562406054, 0)</t>
+  </si>
+  <si>
+    <t>(-9.992458939, 5.954217011, 10)</t>
+  </si>
+  <si>
+    <t>(-5.999999992, 6.504514902, 0)</t>
+  </si>
+  <si>
+    <t>(-2.007540594, 5.954217043, 10)</t>
+  </si>
+  <si>
+    <t>(-10.02127382, 1.555697541, 10)</t>
+  </si>
+  <si>
+    <t>(-5.999999751, 1.538214485, 10)</t>
+  </si>
+  <si>
+    <t>(-1.97872669, 1.555697543, 10)</t>
   </si>
 </sst>
 </file>
@@ -605,8 +1133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57:D58"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1085,4 +1613,1913 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" t="s">
+        <v>5</v>
+      </c>
+      <c r="F20" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C21" t="s">
+        <v>29</v>
+      </c>
+      <c r="E21" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" t="s">
+        <v>78</v>
+      </c>
+      <c r="D27" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>84</v>
+      </c>
+      <c r="B33" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D33" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G39"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:D39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>113</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" t="s">
+        <v>94</v>
+      </c>
+      <c r="G19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>114</v>
+      </c>
+      <c r="B20" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20" t="s">
+        <v>116</v>
+      </c>
+      <c r="E20" t="s">
+        <v>94</v>
+      </c>
+      <c r="F20" t="s">
+        <v>94</v>
+      </c>
+      <c r="G20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>117</v>
+      </c>
+      <c r="B21" t="s">
+        <v>118</v>
+      </c>
+      <c r="C21" t="s">
+        <v>119</v>
+      </c>
+      <c r="E21" t="s">
+        <v>94</v>
+      </c>
+      <c r="F21" t="s">
+        <v>94</v>
+      </c>
+      <c r="G21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>96</v>
+      </c>
+      <c r="B25" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D33" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>111</v>
+      </c>
+      <c r="B37" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D37" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H137"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="D137" sqref="D137"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>113</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="E19" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" t="s">
+        <v>94</v>
+      </c>
+      <c r="G19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>114</v>
+      </c>
+      <c r="B20" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20" t="s">
+        <v>116</v>
+      </c>
+      <c r="E20" t="s">
+        <v>94</v>
+      </c>
+      <c r="F20" t="s">
+        <v>94</v>
+      </c>
+      <c r="G20" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>117</v>
+      </c>
+      <c r="B21" t="s">
+        <v>118</v>
+      </c>
+      <c r="C21" t="s">
+        <v>119</v>
+      </c>
+      <c r="E21" t="s">
+        <v>94</v>
+      </c>
+      <c r="F21" t="s">
+        <v>94</v>
+      </c>
+      <c r="G21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>134</v>
+      </c>
+      <c r="B23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C25" t="s">
+        <v>17</v>
+      </c>
+      <c r="D25" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>96</v>
+      </c>
+      <c r="B29" t="s">
+        <v>52</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D33" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>22</v>
+      </c>
+      <c r="B37" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D37" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B38" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B39" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>111</v>
+      </c>
+      <c r="B41" t="s">
+        <v>52</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D41" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B42" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B43" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>135</v>
+      </c>
+      <c r="B45" t="s">
+        <v>52</v>
+      </c>
+      <c r="C45" t="s">
+        <v>100</v>
+      </c>
+      <c r="D45" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>103</v>
+      </c>
+      <c r="C46" t="s">
+        <v>97</v>
+      </c>
+      <c r="D46" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>98</v>
+      </c>
+      <c r="C47" t="s">
+        <v>99</v>
+      </c>
+      <c r="D47" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B49" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>137</v>
+      </c>
+      <c r="B51" t="s">
+        <v>52</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D51" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B52" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B53" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>20</v>
+      </c>
+      <c r="B55" t="s">
+        <v>52</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="D55" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B56" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B57" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>22</v>
+      </c>
+      <c r="B59" t="s">
+        <v>52</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D59" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B60" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B61" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>111</v>
+      </c>
+      <c r="B63" t="s">
+        <v>52</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D63" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B64" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B65" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>161</v>
+      </c>
+      <c r="B67" t="s">
+        <v>52</v>
+      </c>
+      <c r="C67" t="s">
+        <v>128</v>
+      </c>
+      <c r="D67" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>129</v>
+      </c>
+      <c r="C68" t="s">
+        <v>130</v>
+      </c>
+      <c r="D68" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
+        <v>132</v>
+      </c>
+      <c r="C69" t="s">
+        <v>154</v>
+      </c>
+      <c r="D69" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>137</v>
+      </c>
+      <c r="B73" t="s">
+        <v>52</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D73" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B74" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B75" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>20</v>
+      </c>
+      <c r="B77" t="s">
+        <v>52</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D77" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B78" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B79" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>22</v>
+      </c>
+      <c r="B81" t="s">
+        <v>52</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D81" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B82" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B83" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>111</v>
+      </c>
+      <c r="B85" t="s">
+        <v>52</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D85" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B86" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B87" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>193</v>
+      </c>
+      <c r="B89" t="s">
+        <v>52</v>
+      </c>
+      <c r="C89" t="s">
+        <v>163</v>
+      </c>
+      <c r="D89" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>167</v>
+      </c>
+      <c r="C90" t="s">
+        <v>171</v>
+      </c>
+      <c r="D90" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>179</v>
+      </c>
+      <c r="C91" t="s">
+        <v>183</v>
+      </c>
+      <c r="D91" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>192</v>
+      </c>
+      <c r="B95" t="s">
+        <v>2</v>
+      </c>
+      <c r="C95" t="s">
+        <v>3</v>
+      </c>
+      <c r="D95" t="s">
+        <v>4</v>
+      </c>
+      <c r="F95" t="s">
+        <v>11</v>
+      </c>
+      <c r="G95" t="s">
+        <v>11</v>
+      </c>
+      <c r="H95" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
+        <v>5</v>
+      </c>
+      <c r="C96" t="s">
+        <v>6</v>
+      </c>
+      <c r="D96" t="s">
+        <v>7</v>
+      </c>
+      <c r="F96" t="s">
+        <v>11</v>
+      </c>
+      <c r="G96" t="s">
+        <v>11</v>
+      </c>
+      <c r="H96" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>8</v>
+      </c>
+      <c r="C97" t="s">
+        <v>9</v>
+      </c>
+      <c r="D97" t="s">
+        <v>10</v>
+      </c>
+      <c r="F97" t="s">
+        <v>11</v>
+      </c>
+      <c r="G97" t="s">
+        <v>11</v>
+      </c>
+      <c r="H97" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>134</v>
+      </c>
+      <c r="B99" t="s">
+        <v>52</v>
+      </c>
+      <c r="C99" t="s">
+        <v>17</v>
+      </c>
+      <c r="D99" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
+        <v>17</v>
+      </c>
+      <c r="C100" t="s">
+        <v>17</v>
+      </c>
+      <c r="D100" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>17</v>
+      </c>
+      <c r="C101" t="s">
+        <v>17</v>
+      </c>
+      <c r="D101" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>194</v>
+      </c>
+      <c r="B103" t="s">
+        <v>52</v>
+      </c>
+      <c r="C103" t="s">
+        <v>195</v>
+      </c>
+      <c r="D103" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B104" t="s">
+        <v>196</v>
+      </c>
+      <c r="C104" t="s">
+        <v>198</v>
+      </c>
+      <c r="D104" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
+        <v>197</v>
+      </c>
+      <c r="C105" t="s">
+        <v>199</v>
+      </c>
+      <c r="D105" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>201</v>
+      </c>
+      <c r="B107" t="s">
+        <v>52</v>
+      </c>
+      <c r="C107" t="s">
+        <v>202</v>
+      </c>
+      <c r="D107" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B108" t="s">
+        <v>205</v>
+      </c>
+      <c r="C108" t="s">
+        <v>203</v>
+      </c>
+      <c r="D108" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
+        <v>206</v>
+      </c>
+      <c r="C109" t="s">
+        <v>204</v>
+      </c>
+      <c r="D109" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>193</v>
+      </c>
+      <c r="B111" t="s">
+        <v>52</v>
+      </c>
+      <c r="C111" t="s">
+        <v>163</v>
+      </c>
+      <c r="D111" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B112" t="s">
+        <v>167</v>
+      </c>
+      <c r="C112" t="s">
+        <v>171</v>
+      </c>
+      <c r="D112" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B113" t="s">
+        <v>179</v>
+      </c>
+      <c r="C113" t="s">
+        <v>183</v>
+      </c>
+      <c r="D113" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
+        <v>209</v>
+      </c>
+      <c r="B115" t="s">
+        <v>52</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D115" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B116" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="D116" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B117" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
+        <v>216</v>
+      </c>
+      <c r="B119" t="s">
+        <v>52</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D119" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B120" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B121" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
+        <v>224</v>
+      </c>
+      <c r="B123" t="s">
+        <v>52</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D123" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B124" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B125" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>20</v>
+      </c>
+      <c r="B127" t="s">
+        <v>52</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D127" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B128" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B129" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>22</v>
+      </c>
+      <c r="B131" t="s">
+        <v>52</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D131" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B132" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B133" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>111</v>
+      </c>
+      <c r="B135" t="s">
+        <v>52</v>
+      </c>
+      <c r="C135" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D135" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B136" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C136" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B137" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="C137" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>245</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added unit test project. Added unit tests for explicit Euler and Verlet. Minor changes needed for unit testing. Fixed typos in manual calculations spreadsheet.
</commit_message>
<xml_diff>
--- a/unit_tests_manual_calculations.xlsx
+++ b/unit_tests_manual_calculations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Explicit Euler" sheetId="1" r:id="rId1"/>
@@ -296,15 +296,6 @@
     <t>(-2, 5.023905, 0)</t>
   </si>
   <si>
-    <t>(-10, -8.39950047, 0)</t>
-  </si>
-  <si>
-    <t>(-6, -1.957050042, 0)</t>
-  </si>
-  <si>
-    <t>(-2, -8.33950047, 0)</t>
-  </si>
-  <si>
     <t xml:space="preserve">T0 </t>
   </si>
   <si>
@@ -765,6 +756,15 @@
   </si>
   <si>
     <t>(-1.97872669, 1.555697543, 10)</t>
+  </si>
+  <si>
+    <t>(-10, -0.839950047, 0)</t>
+  </si>
+  <si>
+    <t>(-6, -0.938095042, 0)</t>
+  </si>
+  <si>
+    <t>(-2, -0.839950047, 0)</t>
   </si>
 </sst>
 </file>
@@ -1133,8 +1133,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G17"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1619,8 +1619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1904,13 +1904,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>89</v>
+        <v>243</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>90</v>
+        <v>244</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>91</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -1922,8 +1922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:D39"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2042,10 +2042,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B13" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -2061,7 +2061,7 @@
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -2069,7 +2069,7 @@
         <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -2077,7 +2077,7 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -2086,7 +2086,7 @@
         <v>11</v>
       </c>
       <c r="F19" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G19" t="s">
         <v>11</v>
@@ -2094,58 +2094,58 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B20" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C20" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E20" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F20" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G20" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B21" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C21" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E21" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F21" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G21" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B25" t="s">
         <v>52</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D25" t="s">
         <v>52</v>
@@ -2153,24 +2153,24 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -2181,7 +2181,7 @@
         <v>52</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D29" t="s">
         <v>52</v>
@@ -2189,24 +2189,24 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="D30" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -2217,7 +2217,7 @@
         <v>52</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D33" t="s">
         <v>52</v>
@@ -2225,35 +2225,35 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B37" t="s">
         <v>52</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D37" t="s">
         <v>52</v>
@@ -2261,24 +2261,24 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -2290,7 +2290,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+    <sheetView topLeftCell="A103" workbookViewId="0">
       <selection activeCell="D137" sqref="D137"/>
     </sheetView>
   </sheetViews>
@@ -2413,7 +2413,7 @@
         <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -2429,7 +2429,7 @@
         <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -2437,7 +2437,7 @@
         <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -2445,7 +2445,7 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -2454,7 +2454,7 @@
         <v>11</v>
       </c>
       <c r="F19" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G19" t="s">
         <v>11</v>
@@ -2462,47 +2462,47 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B20" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C20" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E20" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F20" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G20" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B21" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C21" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="E21" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="F21" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="G21" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B23" t="s">
         <v>52</v>
@@ -2538,18 +2538,18 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B29" t="s">
         <v>52</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D29" t="s">
         <v>52</v>
@@ -2557,24 +2557,24 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -2585,7 +2585,7 @@
         <v>52</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D33" t="s">
         <v>52</v>
@@ -2593,24 +2593,24 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="C34" s="1" t="s">
-        <v>105</v>
-      </c>
       <c r="D34" s="1" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -2621,7 +2621,7 @@
         <v>52</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D37" t="s">
         <v>52</v>
@@ -2629,35 +2629,35 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B41" t="s">
         <v>52</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D41" t="s">
         <v>52</v>
@@ -2665,35 +2665,35 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B45" t="s">
         <v>52</v>
       </c>
       <c r="C45" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D45" t="s">
         <v>52</v>
@@ -2701,40 +2701,40 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C46" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D46" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C47" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D47" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B51" t="s">
         <v>52</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D51" t="s">
         <v>52</v>
@@ -2742,24 +2742,24 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -2770,7 +2770,7 @@
         <v>52</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D55" t="s">
         <v>52</v>
@@ -2778,24 +2778,24 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C56" s="1" t="s">
+      <c r="D56" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C57" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D57" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="D57" s="1" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -2806,7 +2806,7 @@
         <v>52</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="D59" t="s">
         <v>52</v>
@@ -2814,35 +2814,35 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B60" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C60" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C60" s="1" t="s">
-        <v>145</v>
-      </c>
       <c r="D60" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B61" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C61" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>156</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B63" t="s">
         <v>52</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D63" t="s">
         <v>52</v>
@@ -2850,35 +2850,35 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B64" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C64" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C64" s="1" t="s">
-        <v>146</v>
-      </c>
       <c r="D64" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B65" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C65" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B67" t="s">
         <v>52</v>
       </c>
       <c r="C67" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D67" t="s">
         <v>52</v>
@@ -2886,40 +2886,40 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C68" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D68" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C69" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D69" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B73" t="s">
         <v>52</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D73" t="s">
         <v>52</v>
@@ -2927,24 +2927,24 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B74" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B75" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2955,7 +2955,7 @@
         <v>52</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D77" t="s">
         <v>52</v>
@@ -2963,24 +2963,24 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B78" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B79" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -2991,7 +2991,7 @@
         <v>52</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D81" t="s">
         <v>52</v>
@@ -2999,35 +2999,35 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B82" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B83" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B85" t="s">
         <v>52</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D85" t="s">
         <v>52</v>
@@ -3035,35 +3035,35 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B86" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B87" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B89" t="s">
         <v>52</v>
       </c>
       <c r="C89" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D89" t="s">
         <v>52</v>
@@ -3071,34 +3071,34 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C90" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D90" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C91" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D91" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B95" t="s">
         <v>2</v>
@@ -3161,7 +3161,7 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B99" t="s">
         <v>52</v>
@@ -3197,13 +3197,13 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B103" t="s">
         <v>52</v>
       </c>
       <c r="C103" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D103" t="s">
         <v>52</v>
@@ -3211,35 +3211,35 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C104" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D104" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C105" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D105" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B107" t="s">
         <v>52</v>
       </c>
       <c r="C107" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D107" t="s">
         <v>52</v>
@@ -3247,35 +3247,35 @@
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C108" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D108" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C109" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D109" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B111" t="s">
         <v>52</v>
       </c>
       <c r="C111" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D111" t="s">
         <v>52</v>
@@ -3283,35 +3283,35 @@
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C112" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D112" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C113" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D113" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="B115" t="s">
         <v>52</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D115" t="s">
         <v>52</v>
@@ -3319,35 +3319,35 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B116" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B117" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B119" t="s">
         <v>52</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D119" t="s">
         <v>52</v>
@@ -3355,35 +3355,35 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B120" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B121" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B123" t="s">
         <v>52</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="D123" t="s">
         <v>52</v>
@@ -3391,24 +3391,24 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B124" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B125" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -3419,7 +3419,7 @@
         <v>52</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D127" t="s">
         <v>52</v>
@@ -3427,24 +3427,24 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B128" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B129" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -3455,7 +3455,7 @@
         <v>52</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D131" t="s">
         <v>52</v>
@@ -3463,35 +3463,35 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B132" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C132" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D132" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B133" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C133" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B135" t="s">
         <v>52</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D135" t="s">
         <v>52</v>
@@ -3499,24 +3499,24 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B136" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C136" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B137" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C137" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final 2 unit tests added
</commit_message>
<xml_diff>
--- a/unit_tests_manual_calculations.xlsx
+++ b/unit_tests_manual_calculations.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12360" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Explicit Euler" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="245">
   <si>
     <t>T0</t>
   </si>
@@ -345,9 +345,6 @@
   </si>
   <si>
     <t>(0, -.468625, 0)</t>
-  </si>
-  <si>
-    <t>(-3.371747425e-7, -4.904987602, 0)</t>
   </si>
   <si>
     <t>(0, -0.9564575523, 0)</t>
@@ -1619,7 +1616,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
@@ -1904,13 +1901,13 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="D35" s="1" t="s">
         <v>244</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -1922,8 +1919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2077,7 +2074,7 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -2094,13 +2091,13 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>110</v>
+      </c>
+      <c r="B20" t="s">
         <v>111</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>112</v>
-      </c>
-      <c r="C20" t="s">
-        <v>113</v>
       </c>
       <c r="E20" t="s">
         <v>91</v>
@@ -2114,13 +2111,13 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>113</v>
+      </c>
+      <c r="B21" t="s">
         <v>114</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>115</v>
-      </c>
-      <c r="C21" t="s">
-        <v>116</v>
       </c>
       <c r="E21" t="s">
         <v>91</v>
@@ -2217,7 +2214,7 @@
         <v>52</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D33" t="s">
         <v>52</v>
@@ -2225,35 +2222,35 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>105</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>106</v>
+        <v>144</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B37" t="s">
         <v>52</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D37" t="s">
         <v>52</v>
@@ -2261,24 +2258,24 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D38" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D39" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -2445,7 +2442,7 @@
         <v>2</v>
       </c>
       <c r="B19" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -2462,13 +2459,13 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>110</v>
+      </c>
+      <c r="B20" t="s">
         <v>111</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>112</v>
-      </c>
-      <c r="C20" t="s">
-        <v>113</v>
       </c>
       <c r="E20" t="s">
         <v>91</v>
@@ -2482,13 +2479,13 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>113</v>
+      </c>
+      <c r="B21" t="s">
         <v>114</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>115</v>
-      </c>
-      <c r="C21" t="s">
-        <v>116</v>
       </c>
       <c r="E21" t="s">
         <v>91</v>
@@ -2502,7 +2499,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B23" t="s">
         <v>52</v>
@@ -2621,7 +2618,7 @@
         <v>52</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D37" t="s">
         <v>52</v>
@@ -2629,35 +2626,35 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>105</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B41" t="s">
         <v>52</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D41" t="s">
         <v>52</v>
@@ -2665,29 +2662,29 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D42" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B45" t="s">
         <v>52</v>
@@ -2723,18 +2720,18 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B51" t="s">
         <v>52</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D51" t="s">
         <v>52</v>
@@ -2742,24 +2739,24 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C52" s="1" t="s">
+      <c r="D52" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -2770,7 +2767,7 @@
         <v>52</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D55" t="s">
         <v>52</v>
@@ -2778,24 +2775,24 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -2806,7 +2803,7 @@
         <v>52</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D59" t="s">
         <v>52</v>
@@ -2814,35 +2811,35 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B60" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B61" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B63" t="s">
         <v>52</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D63" t="s">
         <v>52</v>
@@ -2850,35 +2847,35 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B64" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B65" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B67" t="s">
         <v>52</v>
       </c>
       <c r="C67" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D67" t="s">
         <v>52</v>
@@ -2886,40 +2883,40 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
+        <v>125</v>
+      </c>
+      <c r="C68" t="s">
         <v>126</v>
       </c>
-      <c r="C68" t="s">
+      <c r="D68" t="s">
         <v>127</v>
-      </c>
-      <c r="D68" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B69" t="s">
+        <v>128</v>
+      </c>
+      <c r="C69" t="s">
+        <v>150</v>
+      </c>
+      <c r="D69" t="s">
         <v>129</v>
-      </c>
-      <c r="C69" t="s">
-        <v>151</v>
-      </c>
-      <c r="D69" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B71" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B73" t="s">
         <v>52</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D73" t="s">
         <v>52</v>
@@ -2927,24 +2924,24 @@
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B74" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B75" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2955,7 +2952,7 @@
         <v>52</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D77" t="s">
         <v>52</v>
@@ -2963,24 +2960,24 @@
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B78" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B79" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -2991,7 +2988,7 @@
         <v>52</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D81" t="s">
         <v>52</v>
@@ -2999,35 +2996,35 @@
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B82" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B83" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B85" t="s">
         <v>52</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D85" t="s">
         <v>52</v>
@@ -3035,35 +3032,35 @@
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B86" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B87" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B89" t="s">
         <v>52</v>
       </c>
       <c r="C89" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D89" t="s">
         <v>52</v>
@@ -3071,34 +3068,34 @@
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C90" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D90" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C91" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D91" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B95" t="s">
         <v>2</v>
@@ -3161,7 +3158,7 @@
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B99" t="s">
         <v>52</v>
@@ -3197,13 +3194,13 @@
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
+        <v>190</v>
+      </c>
+      <c r="B103" t="s">
+        <v>52</v>
+      </c>
+      <c r="C103" t="s">
         <v>191</v>
-      </c>
-      <c r="B103" t="s">
-        <v>52</v>
-      </c>
-      <c r="C103" t="s">
-        <v>192</v>
       </c>
       <c r="D103" t="s">
         <v>52</v>
@@ -3211,35 +3208,35 @@
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B104" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C104" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D104" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C105" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D105" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
+        <v>197</v>
+      </c>
+      <c r="B107" t="s">
+        <v>52</v>
+      </c>
+      <c r="C107" t="s">
         <v>198</v>
-      </c>
-      <c r="B107" t="s">
-        <v>52</v>
-      </c>
-      <c r="C107" t="s">
-        <v>199</v>
       </c>
       <c r="D107" t="s">
         <v>52</v>
@@ -3247,35 +3244,35 @@
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B108" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C108" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D108" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B109" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C109" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D109" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B111" t="s">
         <v>52</v>
       </c>
       <c r="C111" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D111" t="s">
         <v>52</v>
@@ -3283,35 +3280,35 @@
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B112" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C112" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D112" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C113" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D113" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
+        <v>205</v>
+      </c>
+      <c r="B115" t="s">
+        <v>52</v>
+      </c>
+      <c r="C115" s="1" t="s">
         <v>206</v>
-      </c>
-      <c r="B115" t="s">
-        <v>52</v>
-      </c>
-      <c r="C115" s="1" t="s">
-        <v>207</v>
       </c>
       <c r="D115" t="s">
         <v>52</v>
@@ -3319,35 +3316,35 @@
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B116" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="C116" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="C116" s="1" t="s">
+      <c r="D116" s="1" t="s">
         <v>209</v>
-      </c>
-      <c r="D116" s="1" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B117" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C117" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="C117" s="1" t="s">
-        <v>212</v>
-      </c>
       <c r="D117" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
+        <v>212</v>
+      </c>
+      <c r="B119" t="s">
+        <v>52</v>
+      </c>
+      <c r="C119" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="B119" t="s">
-        <v>52</v>
-      </c>
-      <c r="C119" s="1" t="s">
-        <v>214</v>
       </c>
       <c r="D119" t="s">
         <v>52</v>
@@ -3355,35 +3352,35 @@
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B120" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C120" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="C120" s="1" t="s">
+      <c r="D120" s="1" t="s">
         <v>216</v>
-      </c>
-      <c r="D120" s="1" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B121" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="C121" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="C121" s="1" t="s">
+      <c r="D121" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="D121" s="1" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
+        <v>220</v>
+      </c>
+      <c r="B123" t="s">
+        <v>52</v>
+      </c>
+      <c r="C123" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="B123" t="s">
-        <v>52</v>
-      </c>
-      <c r="C123" s="1" t="s">
-        <v>222</v>
       </c>
       <c r="D123" t="s">
         <v>52</v>
@@ -3391,24 +3388,24 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B124" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C124" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="C124" s="1" t="s">
+      <c r="D124" s="1" t="s">
         <v>224</v>
-      </c>
-      <c r="D124" s="1" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B125" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="C125" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="C125" s="1" t="s">
+      <c r="D125" s="1" t="s">
         <v>227</v>
-      </c>
-      <c r="D125" s="1" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
@@ -3419,7 +3416,7 @@
         <v>52</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D127" t="s">
         <v>52</v>
@@ -3427,24 +3424,24 @@
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B128" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C128" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="C128" s="1" t="s">
+      <c r="D128" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="D128" s="1" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B129" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C129" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="C129" s="1" t="s">
+      <c r="D129" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="D129" s="1" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -3455,7 +3452,7 @@
         <v>52</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D131" t="s">
         <v>52</v>
@@ -3463,35 +3460,35 @@
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B132" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="C132" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="C132" s="1" t="s">
+      <c r="D132" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="D132" s="1" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B133" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C133" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="C133" s="1" t="s">
+      <c r="D133" s="1" t="s">
         <v>234</v>
-      </c>
-      <c r="D133" s="1" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B135" t="s">
         <v>52</v>
       </c>
       <c r="C135" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D135" t="s">
         <v>52</v>
@@ -3499,24 +3496,24 @@
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B136" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C136" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="C136" s="1" t="s">
+      <c r="D136" s="1" t="s">
         <v>238</v>
-      </c>
-      <c r="D136" s="1" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B137" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="C137" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="C137" s="1" t="s">
+      <c r="D137" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="D137" s="1" t="s">
-        <v>242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>